<commit_message>
Label the trajectories by Mahdi
</commit_message>
<xml_diff>
--- a/tools/labels.xlsx
+++ b/tools/labels.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr date1904="false" showObjects="all" backupFile="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr fullCalcOnLoad="true" refMode="A1" iterate="false" iterateCount="100" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="377">
   <si>
     <t xml:space="preserve">images</t>
   </si>
@@ -1136,6 +1136,21 @@
   </si>
   <si>
     <t xml:space="preserve">jurkat_I22.mat_Set87_TrId14.png</t>
+  </si>
+  <si>
+    <t>Mahdi</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>neg</t>
+  </si>
+  <si>
+    <t>unsure</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="797">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1186,6 +1201,802 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1212,7 +2023,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="800">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1229,6 +2040,802 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="71" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="72" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="73" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="74" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="75" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="85" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="88" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="89" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="90" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="91" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="92" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="93" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="94" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="95" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="96" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="97" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="98" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="99" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="100" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="101" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="102" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="103" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="104" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="105" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="106" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="109" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="110" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="111" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="112" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="113" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="114" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="115" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="116" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="117" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="120" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="121" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="122" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="123" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="124" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="125" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="126" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="127" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="129" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="131" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="132" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="133" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="137" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="138" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="139" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="143" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="144" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="145" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="146" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="147" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="148" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="149" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="150" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="159" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="160" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="166" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="167" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="170" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="171" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="173" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="174" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="180" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="181" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="184" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="185" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="186" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="187" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="188" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="189" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="190" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="191" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="192" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="193" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="194" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="195" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="196" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="197" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="198" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="199" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="200" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="201" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="202" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="203" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="204" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="205" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="206" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="207" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="208" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="209" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="210" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="211" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="212" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="213" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="214" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="215" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="216" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="217" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="218" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="219" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="220" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="221" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="222" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="223" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="224" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="225" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="226" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="227" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="228" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="229" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="230" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="231" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="232" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="233" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="234" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="235" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="236" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="237" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="238" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="239" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="240" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="241" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="242" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="243" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="244" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="245" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="246" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="247" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="248" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="249" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="250" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="251" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="267" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="268" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="269" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="270" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="274" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="275" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="276" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="277" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="278" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="279" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="280" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="281" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="282" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="283" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="284" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="285" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="286" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="287" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="288" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="289" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="290" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="291" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="292" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="293" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="294" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="295" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="296" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="297" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="300" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="301" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="302" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="303" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="304" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="305" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="306" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="307" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="308" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="309" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="310" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="311" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="312" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="313" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="314" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="315" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="316" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="317" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="318" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="319" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="320" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="321" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="322" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="323" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="324" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="325" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="326" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="327" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="328" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="329" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="330" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="331" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="332" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="333" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="334" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="335" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="336" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="337" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="338" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="339" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="340" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="341" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="342" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="343" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="344" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="345" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="346" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="347" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="348" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="349" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="350" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="351" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="352" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="353" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="354" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="355" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="356" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="357" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="358" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="359" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="360" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="361" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="362" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="363" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="364" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="365" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="366" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="367" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="368" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="369" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="370" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="371" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="372" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="373" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="374" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="375" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="376" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="377" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="378" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="379" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="380" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="381" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="382" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="383" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="384" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="385" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="386" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="387" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="388" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="389" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="390" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="391" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="392" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="393" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="394" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="395" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="396" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="397" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="398" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="399" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="400" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="401" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="402" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="403" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="404" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="405" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="406" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="407" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="408" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="409" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="410" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="411" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="412" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="413" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="414" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="415" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="416" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="417" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="418" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="419" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="420" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="421" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="422" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="423" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="424" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="425" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="426" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="427" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="428" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="429" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="430" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="431" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="432" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="433" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="434" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="435" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="436" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="437" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="438" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="439" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="440" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="441" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="442" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="443" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="444" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="445" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="446" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="447" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="448" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="449" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="450" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="451" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="452" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="453" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="454" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="455" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="456" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="457" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="458" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="459" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="460" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="461" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="462" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="463" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="464" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="465" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="466" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="467" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="468" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="469" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="470" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="471" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="472" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="473" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="474" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="475" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="476" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="477" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="478" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="479" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="480" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="481" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="482" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="483" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="484" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="485" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="486" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="487" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="488" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="489" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="490" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="491" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="492" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="493" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="494" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="495" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="496" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="497" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="498" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="499" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="500" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="501" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="502" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="503" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="504" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="505" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="506" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="507" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="508" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="509" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="510" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="511" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="512" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="513" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="514" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="515" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="516" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="517" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="518" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="519" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="520" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="521" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="522" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="523" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="524" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="525" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="526" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="527" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="528" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="529" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="530" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="531" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="532" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="533" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="534" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="535" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="536" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="537" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="538" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="539" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="540" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="541" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="542" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="543" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="544" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="545" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="546" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="547" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="548" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="549" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="550" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="551" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="552" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="553" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="554" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="555" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="556" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="557" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="558" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="559" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="560" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="561" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="562" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="563" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="564" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="565" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="566" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="567" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="568" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="569" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="570" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="571" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="572" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="573" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="574" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="575" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="576" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="577" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="578" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="579" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="580" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="581" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="582" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="583" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="584" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="585" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="586" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="587" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="588" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="589" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="590" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="591" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="592" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="593" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="594" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="595" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="596" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="597" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="598" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="599" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="600" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="601" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="602" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="603" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="604" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="605" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="606" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="607" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="608" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="609" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="610" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="611" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="612" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="613" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="614" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="615" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="616" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="617" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="618" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="619" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="620" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="621" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="622" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="623" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="624" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="625" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="626" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="627" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="628" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="629" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="630" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="631" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="632" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="633" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="634" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="635" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="636" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="637" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="638" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="639" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="640" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="641" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="642" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="643" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="644" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="645" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="646" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="647" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="648" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="649" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="650" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="651" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="652" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="653" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="654" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="655" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="656" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="657" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="658" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="659" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="660" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="661" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="662" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="663" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="664" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="665" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="666" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="667" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="668" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="669" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="670" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="671" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="672" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="673" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="674" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="675" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="676" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="677" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="678" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="679" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="680" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="681" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="682" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="683" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="684" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="685" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="686" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="687" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="688" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="689" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="690" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="691" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="692" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="693" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="694" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="695" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="696" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="697" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="698" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="699" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="700" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="701" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="702" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="703" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="704" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="705" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="706" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="707" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="708" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="709" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="710" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="711" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="712" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="713" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="714" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="715" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="716" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="717" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="718" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="719" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="720" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="721" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="722" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="723" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="724" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="725" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="726" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="727" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="728" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="729" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="730" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="731" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="732" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="733" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="734" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="735" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="736" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="737" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="738" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="739" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="740" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="741" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="742" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="743" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="744" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="745" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="746" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="747" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="748" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="749" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="750" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="751" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="752" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="753" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="754" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="755" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="756" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="757" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="758" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="759" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="760" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="761" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="762" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="763" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="764" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="765" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="766" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="767" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="768" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="769" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="770" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="771" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="772" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="773" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="774" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="775" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="776" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="777" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="778" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="779" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="780" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="781" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="782" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="783" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="784" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="785" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="786" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="787" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="788" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="789" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="790" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="791" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="792" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="793" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="794" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="795" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="796" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1254,13 +2861,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="7"/>
+    <col min="1" max="1" width="43.36" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="2" max="2" width="7.28" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="3" max="3" width="7.28" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="4" max="4" width="6.6015625" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="6" max="6" width="4.46" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="7" max="7" width="4.18" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="8" max="9" width="7" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,7 +2880,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="4" t="s">
+        <v>372</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1286,7 +2895,9 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="1"/>
+      <c r="D2" s="6" t="s">
+        <v>373</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1299,7 +2910,9 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="756" t="s">
+        <v>373</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1312,7 +2925,9 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="10" t="s">
+        <v>374</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1325,7 +2940,9 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="12" t="s">
+        <v>375</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1338,7 +2955,9 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="14" t="s">
+        <v>373</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1351,7 +2970,9 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="16" t="s">
+        <v>373</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1364,2076 +2985,3165 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
+      <c r="D8" s="752" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="3"/>
+      <c r="D9" s="758" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="3"/>
+      <c r="D10" s="22" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="3"/>
+      <c r="D11" s="24" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="3"/>
+      <c r="D12" s="26" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="3"/>
+      <c r="D13" s="28" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="3"/>
+      <c r="D14" s="30" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="3"/>
+      <c r="D15" s="32" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="3"/>
+      <c r="D16" s="760" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="3"/>
+      <c r="D17" s="36" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="3"/>
+      <c r="D18" s="38" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="3"/>
+      <c r="D19" s="40" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="3"/>
+      <c r="D20" s="42" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="3"/>
+      <c r="D21" s="44" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="3"/>
+      <c r="D22" s="46" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="3"/>
+      <c r="D23" s="48" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="3"/>
+      <c r="D24" s="50" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="3"/>
+      <c r="D25" s="52" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="3"/>
+      <c r="D26" s="54" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="3"/>
+      <c r="D27" s="56" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="3"/>
+      <c r="D28" s="58" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="3"/>
+      <c r="D29" s="60" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="3"/>
+      <c r="D30" s="762" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="3"/>
+      <c r="D31" s="64" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="3"/>
+      <c r="D32" s="66" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="3"/>
+      <c r="D33" s="68" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="3"/>
+      <c r="D34" s="764" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="3"/>
+      <c r="D35" s="72" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="3"/>
+      <c r="D36" s="74" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="3"/>
+      <c r="D37" s="76" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="3"/>
+      <c r="D38" s="78" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B39" s="3"/>
+      <c r="D39" s="80" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B40" s="3"/>
+      <c r="D40" s="82" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="3"/>
+      <c r="D41" s="84" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="3"/>
+      <c r="D42" s="86" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B43" s="3"/>
+      <c r="D43" s="88" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B44" s="3"/>
+      <c r="D44" s="90" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="3"/>
+      <c r="D45" s="92" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B46" s="3"/>
+      <c r="D46" s="94" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B47" s="3"/>
+      <c r="D47" s="96" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B48" s="3"/>
+      <c r="D48" s="98" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B49" s="3"/>
+      <c r="D49" s="100" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B50" s="3"/>
+      <c r="D50" s="102" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B51" s="3"/>
+      <c r="D51" s="104" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="3"/>
+      <c r="D52" s="106" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B53" s="3"/>
+      <c r="D53" s="766" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B54" s="3"/>
+      <c r="D54" s="110" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="3"/>
+      <c r="D55" s="112" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B56" s="3"/>
+      <c r="D56" s="114" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B57" s="3"/>
+      <c r="D57" s="116" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B58" s="3"/>
+      <c r="D58" s="118" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B59" s="3"/>
+      <c r="D59" s="120" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B60" s="3"/>
+      <c r="D60" s="122" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B61" s="3"/>
+      <c r="D61" s="124" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B62" s="3"/>
+      <c r="D62" s="126" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B63" s="3"/>
+      <c r="D63" s="128" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B64" s="3"/>
+      <c r="D64" s="130" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B65" s="3"/>
+      <c r="D65" s="132" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B66" s="3"/>
+      <c r="D66" s="134" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B67" s="3"/>
+      <c r="D67" s="136" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B68" s="3"/>
+      <c r="D68" s="138" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B69" s="3"/>
+      <c r="D69" s="140" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B70" s="3"/>
+      <c r="D70" s="142" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B71" s="3"/>
+      <c r="D71" s="144" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B72" s="3"/>
+      <c r="D72" s="146" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B73" s="3"/>
+      <c r="D73" s="148" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B74" s="3"/>
+      <c r="D74" s="150" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B75" s="3"/>
+      <c r="D75" s="152" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B76" s="3"/>
+      <c r="D76" s="154" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B77" s="3"/>
+      <c r="D77" s="156" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B78" s="3"/>
+      <c r="D78" s="158" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B79" s="3"/>
+      <c r="D79" s="160" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B80" s="3"/>
+      <c r="D80" s="162" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B81" s="3"/>
+      <c r="D81" s="164" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B82" s="3"/>
+      <c r="D82" s="166" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B83" s="3"/>
+      <c r="D83" s="168" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B84" s="3"/>
+      <c r="D84" s="170" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B85" s="3"/>
+      <c r="D85" s="172" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B86" s="3"/>
+      <c r="D86" s="174" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B87" s="3"/>
+      <c r="D87" s="176" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B88" s="3"/>
+      <c r="D88" s="178" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B89" s="3"/>
+      <c r="D89" s="180" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B90" s="3"/>
+      <c r="D90" s="182" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B91" s="3"/>
+      <c r="D91" s="184" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B92" s="3"/>
+      <c r="D92" s="186" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B93" s="3"/>
+      <c r="D93" s="768" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B94" s="3"/>
+      <c r="D94" s="190" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B95" s="3"/>
+      <c r="D95" s="192" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B96" s="3"/>
+      <c r="D96" s="194" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B97" s="3"/>
+      <c r="D97" s="196" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B98" s="3"/>
+      <c r="D98" s="198" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B99" s="3"/>
+      <c r="D99" s="200" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B100" s="3"/>
+      <c r="D100" s="202" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B101" s="3"/>
+      <c r="D101" s="204" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B102" s="3"/>
+      <c r="D102" s="770" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B103" s="3"/>
+      <c r="D103" s="208" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B104" s="3"/>
+      <c r="D104" s="210" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B105" s="3"/>
+      <c r="D105" s="212" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B106" s="3"/>
+      <c r="D106" s="214" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B107" s="3"/>
+      <c r="D107" s="216" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B108" s="3"/>
+      <c r="D108" s="218" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B109" s="3"/>
+      <c r="D109" s="220" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B110" s="3"/>
+      <c r="D110" s="222" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B111" s="3"/>
+      <c r="D111" s="224" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B112" s="3"/>
+      <c r="D112" s="226" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B113" s="3"/>
+      <c r="D113" s="228" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B114" s="3"/>
+      <c r="D114" s="230" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B115" s="3"/>
+      <c r="D115" s="232" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B116" s="3"/>
+      <c r="D116" s="234" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B117" s="3"/>
+      <c r="D117" s="236" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B118" s="3"/>
+      <c r="D118" s="238" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B119" s="3"/>
+      <c r="D119" s="240" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B120" s="3"/>
+      <c r="D120" s="242" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B121" s="3"/>
+      <c r="D121" s="244" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B122" s="3"/>
+      <c r="D122" s="246" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B123" s="3"/>
+      <c r="D123" s="772" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B124" s="3"/>
+      <c r="D124" s="250" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B125" s="3"/>
+      <c r="D125" s="252" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B126" s="3"/>
+      <c r="D126" s="774" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B127" s="3"/>
+      <c r="D127" s="256" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B128" s="3"/>
+      <c r="D128" s="258" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B129" s="3"/>
+      <c r="D129" s="260" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="130" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B130" s="3"/>
+      <c r="D130" s="776" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B131" s="3"/>
+      <c r="D131" s="264" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B132" s="3"/>
+      <c r="D132" s="266" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B133" s="3"/>
+      <c r="D133" s="268" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B134" s="3"/>
+      <c r="D134" s="270" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B135" s="3"/>
+      <c r="D135" s="272" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B136" s="3"/>
+      <c r="D136" s="274" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B137" s="3"/>
+      <c r="D137" s="276" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B138" s="3"/>
+      <c r="D138" s="278" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B139" s="3"/>
+      <c r="D139" s="280" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B140" s="3"/>
+      <c r="D140" s="282" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B141" s="3"/>
+      <c r="D141" s="284" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B142" s="3"/>
+      <c r="D142" s="286" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B143" s="3"/>
+      <c r="D143" s="288" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B144" s="3"/>
+      <c r="D144" s="290" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B145" s="3"/>
+      <c r="D145" s="778" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B146" s="3"/>
+      <c r="D146" s="294" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B147" s="3"/>
+      <c r="D147" s="296" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B148" s="3"/>
+      <c r="D148" s="298" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B149" s="3"/>
+      <c r="D149" s="300" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B150" s="3"/>
+      <c r="D150" s="302" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="151" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="2" t="s">
         <v>152</v>
       </c>
       <c r="B151" s="3"/>
+      <c r="D151" s="304" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B152" s="3"/>
+      <c r="D152" s="306" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="153" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B153" s="3"/>
+      <c r="D153" s="308" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B154" s="3"/>
+      <c r="D154" s="310" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="155" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B155" s="3"/>
+      <c r="D155" s="780" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B156" s="3"/>
+      <c r="D156" s="316" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B157" s="3"/>
+      <c r="D157" s="318" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="s">
         <v>159</v>
       </c>
       <c r="B158" s="3"/>
+      <c r="D158" s="320" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B159" s="3"/>
+      <c r="D159" s="322" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="160" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="s">
         <v>161</v>
       </c>
       <c r="B160" s="3"/>
+      <c r="D160" s="324" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B161" s="3"/>
+      <c r="D161" s="326" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="162" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B162" s="3"/>
+      <c r="D162" s="328" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="s">
         <v>164</v>
       </c>
       <c r="B163" s="3"/>
+      <c r="D163" s="330" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="164" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="2" t="s">
         <v>165</v>
       </c>
       <c r="B164" s="3"/>
+      <c r="D164" s="332" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B165" s="3"/>
+      <c r="D165" s="782" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="166" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="s">
         <v>167</v>
       </c>
       <c r="B166" s="3"/>
+      <c r="D166" s="336" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B167" s="3"/>
+      <c r="D167" s="338" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="168" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="2" t="s">
         <v>169</v>
       </c>
       <c r="B168" s="3"/>
+      <c r="D168" s="340" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="169" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B169" s="3"/>
+      <c r="D169" s="342" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="170" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="2" t="s">
         <v>171</v>
       </c>
       <c r="B170" s="3"/>
+      <c r="D170" s="344" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="171" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B171" s="3"/>
+      <c r="D171" s="346" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="172" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B172" s="3"/>
+      <c r="D172" s="348" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="s">
         <v>174</v>
       </c>
       <c r="B173" s="3"/>
+      <c r="D173" s="350" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B174" s="3"/>
+      <c r="D174" s="352" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="175" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B175" s="3"/>
+      <c r="D175" s="354" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="2" t="s">
         <v>177</v>
       </c>
       <c r="B176" s="3"/>
+      <c r="D176" s="356" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B177" s="3"/>
+      <c r="D177" s="358" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B178" s="3"/>
+      <c r="D178" s="360" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B179" s="3"/>
+      <c r="D179" s="784" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="180" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B180" s="3"/>
+      <c r="D180" s="364" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B181" s="3"/>
+      <c r="D181" s="366" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="182" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
         <v>183</v>
       </c>
       <c r="B182" s="3"/>
+      <c r="D182" s="368" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B183" s="3"/>
+      <c r="D183" s="370" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="184" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B184" s="3"/>
+      <c r="D184" s="372" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="185" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B185" s="3"/>
+      <c r="D185" s="374" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="186" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B186" s="3"/>
+      <c r="D186" s="376" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="187" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B187" s="3"/>
+      <c r="D187" s="786" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="188" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B188" s="3"/>
+      <c r="D188" s="380" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B189" s="3"/>
+      <c r="D189" s="382" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="190" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
         <v>191</v>
       </c>
       <c r="B190" s="3"/>
+      <c r="D190" s="384" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="191" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B191" s="3"/>
+      <c r="D191" s="386" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="2" t="s">
         <v>193</v>
       </c>
       <c r="B192" s="3"/>
+      <c r="D192" s="388" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="193" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="s">
         <v>194</v>
       </c>
       <c r="B193" s="3"/>
+      <c r="D193" s="390" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="194" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="2" t="s">
         <v>195</v>
       </c>
       <c r="B194" s="3"/>
+      <c r="D194" s="392" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="195" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B195" s="3"/>
+      <c r="D195" s="394" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="196" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="s">
         <v>197</v>
       </c>
       <c r="B196" s="3"/>
+      <c r="D196" s="396" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="197" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B197" s="3"/>
+      <c r="D197" s="398" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="198" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="2" t="s">
         <v>199</v>
       </c>
       <c r="B198" s="3"/>
+      <c r="D198" s="400" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="199" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="2" t="s">
         <v>200</v>
       </c>
       <c r="B199" s="3"/>
+      <c r="D199" s="402" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="200" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="2" t="s">
         <v>201</v>
       </c>
       <c r="B200" s="3"/>
+      <c r="D200" s="404" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="201" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B201" s="3"/>
+      <c r="D201" s="406" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="202" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B202" s="3"/>
+      <c r="D202" s="408" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="203" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B203" s="3"/>
+      <c r="D203" s="410" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="204" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="2" t="s">
         <v>205</v>
       </c>
       <c r="B204" s="3"/>
+      <c r="D204" s="412" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="205" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="2" t="s">
         <v>206</v>
       </c>
       <c r="B205" s="3"/>
+      <c r="D205" s="414" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="206" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="2" t="s">
         <v>207</v>
       </c>
       <c r="B206" s="3"/>
+      <c r="D206" s="416" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="207" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="2" t="s">
         <v>208</v>
       </c>
       <c r="B207" s="3"/>
+      <c r="D207" s="418" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="208" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="2" t="s">
         <v>209</v>
       </c>
       <c r="B208" s="3"/>
+      <c r="D208" s="420" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="209" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="2" t="s">
         <v>210</v>
       </c>
       <c r="B209" s="3"/>
+      <c r="D209" s="422" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="210" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="2" t="s">
         <v>211</v>
       </c>
       <c r="B210" s="3"/>
+      <c r="D210" s="424" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="211" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="2" t="s">
         <v>212</v>
       </c>
       <c r="B211" s="3"/>
+      <c r="D211" s="426" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="212" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="2" t="s">
         <v>213</v>
       </c>
       <c r="B212" s="3"/>
+      <c r="D212" s="428" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="213" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B213" s="3"/>
+      <c r="D213" s="430" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="214" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="2" t="s">
         <v>215</v>
       </c>
       <c r="B214" s="3"/>
+      <c r="D214" s="432" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="215" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="2" t="s">
         <v>216</v>
       </c>
       <c r="B215" s="3"/>
+      <c r="D215" s="434" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="216" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="2" t="s">
         <v>217</v>
       </c>
       <c r="B216" s="3"/>
+      <c r="D216" s="436" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="217" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="2" t="s">
         <v>218</v>
       </c>
       <c r="B217" s="3"/>
+      <c r="D217" s="438" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="218" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="2" t="s">
         <v>219</v>
       </c>
       <c r="B218" s="3"/>
+      <c r="D218" s="440" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="219" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B219" s="3"/>
+      <c r="D219" s="442" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="220" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="2" t="s">
         <v>221</v>
       </c>
       <c r="B220" s="3"/>
+      <c r="D220" s="788" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="221" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="s">
         <v>222</v>
       </c>
       <c r="B221" s="3"/>
+      <c r="D221" s="446" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="222" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="2" t="s">
         <v>223</v>
       </c>
       <c r="B222" s="3"/>
+      <c r="D222" s="448" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="223" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="2" t="s">
         <v>224</v>
       </c>
       <c r="B223" s="3"/>
+      <c r="D223" s="450" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="224" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="2" t="s">
         <v>225</v>
       </c>
       <c r="B224" s="3"/>
+      <c r="D224" s="452" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="225" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="2" t="s">
         <v>226</v>
       </c>
       <c r="B225" s="3"/>
+      <c r="D225" s="454" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="226" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="2" t="s">
         <v>227</v>
       </c>
       <c r="B226" s="3"/>
+      <c r="D226" s="456" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="227" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="2" t="s">
         <v>228</v>
       </c>
       <c r="B227" s="3"/>
+      <c r="D227" s="458" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="228" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="2" t="s">
         <v>229</v>
       </c>
       <c r="B228" s="3"/>
+      <c r="D228" s="460" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="229" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="2" t="s">
         <v>230</v>
       </c>
       <c r="B229" s="3"/>
+      <c r="D229" s="462" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="230" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B230" s="3"/>
+      <c r="D230" s="464" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="231" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="2" t="s">
         <v>232</v>
       </c>
       <c r="B231" s="3"/>
+      <c r="D231" s="466" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="232" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="2" t="s">
         <v>233</v>
       </c>
       <c r="B232" s="3"/>
+      <c r="D232" s="468" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="233" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="2" t="s">
         <v>234</v>
       </c>
       <c r="B233" s="3"/>
+      <c r="D233" s="470" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="234" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="2" t="s">
         <v>235</v>
       </c>
       <c r="B234" s="3"/>
+      <c r="D234" s="472" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="235" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="2" t="s">
         <v>236</v>
       </c>
       <c r="B235" s="3"/>
+      <c r="D235" s="474" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="236" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="2" t="s">
         <v>237</v>
       </c>
       <c r="B236" s="3"/>
+      <c r="D236" s="476" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="237" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
         <v>238</v>
       </c>
       <c r="B237" s="3"/>
+      <c r="D237" s="790" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="238" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
         <v>239</v>
       </c>
       <c r="B238" s="3"/>
+      <c r="D238" s="480" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="239" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
         <v>240</v>
       </c>
       <c r="B239" s="3"/>
+      <c r="D239" s="482" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="240" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
         <v>241</v>
       </c>
       <c r="B240" s="3"/>
+      <c r="D240" s="484" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="241" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B241" s="3"/>
+      <c r="D241" s="486" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="242" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
         <v>243</v>
       </c>
       <c r="B242" s="3"/>
+      <c r="D242" s="488" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="243" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
         <v>244</v>
       </c>
       <c r="B243" s="3"/>
+      <c r="D243" s="490" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="244" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
         <v>245</v>
       </c>
       <c r="B244" s="3"/>
+      <c r="D244" s="492" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="245" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
         <v>246</v>
       </c>
       <c r="B245" s="3"/>
+      <c r="D245" s="494" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="246" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
         <v>247</v>
       </c>
       <c r="B246" s="3"/>
+      <c r="D246" s="496" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="247" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
         <v>248</v>
       </c>
       <c r="B247" s="3"/>
+      <c r="D247" s="498" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="248" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
         <v>249</v>
       </c>
       <c r="B248" s="3"/>
+      <c r="D248" s="500" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="249" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
         <v>250</v>
       </c>
       <c r="B249" s="3"/>
+      <c r="D249" s="502" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="250" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
         <v>251</v>
       </c>
       <c r="B250" s="3"/>
+      <c r="D250" s="504" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="251" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
         <v>252</v>
       </c>
       <c r="B251" s="3"/>
+      <c r="D251" s="506" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="252" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
         <v>253</v>
       </c>
       <c r="B252" s="3"/>
+      <c r="D252" s="508" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="253" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
         <v>254</v>
       </c>
       <c r="B253" s="3"/>
+      <c r="D253" s="510" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="254" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="s">
         <v>255</v>
       </c>
       <c r="B254" s="3"/>
+      <c r="D254" s="512" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="255" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
         <v>256</v>
       </c>
       <c r="B255" s="3"/>
+      <c r="D255" s="514" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="256" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="s">
         <v>257</v>
       </c>
       <c r="B256" s="3"/>
+      <c r="D256" s="516" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="257" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B257" s="3"/>
+      <c r="D257" s="518" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="258" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="2" t="s">
         <v>259</v>
       </c>
       <c r="B258" s="3"/>
+      <c r="D258" s="520" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="259" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="2" t="s">
         <v>260</v>
       </c>
       <c r="B259" s="3"/>
+      <c r="D259" s="522" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="260" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="2" t="s">
         <v>261</v>
       </c>
       <c r="B260" s="3"/>
+      <c r="D260" s="524" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="261" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="2" t="s">
         <v>262</v>
       </c>
       <c r="B261" s="3"/>
+      <c r="D261" s="526" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="262" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
         <v>263</v>
       </c>
       <c r="B262" s="3"/>
+      <c r="D262" s="528" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="263" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="s">
         <v>264</v>
       </c>
       <c r="B263" s="3"/>
+      <c r="D263" s="530" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="264" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="2" t="s">
         <v>265</v>
       </c>
       <c r="B264" s="3"/>
+      <c r="D264" s="532" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="265" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="2" t="s">
         <v>266</v>
       </c>
       <c r="B265" s="3"/>
+      <c r="D265" s="534" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="266" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="2" t="s">
         <v>267</v>
       </c>
       <c r="B266" s="3"/>
+      <c r="D266" s="536" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="267" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="2" t="s">
         <v>268</v>
       </c>
       <c r="B267" s="3"/>
+      <c r="D267" s="538" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="268" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
         <v>269</v>
       </c>
       <c r="B268" s="3"/>
+      <c r="D268" s="540" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="269" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="2" t="s">
         <v>270</v>
       </c>
+      <c r="D269" s="542" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="270" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
         <v>271</v>
       </c>
+      <c r="D270" s="544" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="271" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="2" t="s">
         <v>272</v>
       </c>
+      <c r="D271" s="546" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="272" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="2" t="s">
         <v>273</v>
       </c>
+      <c r="D272" s="548" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="273" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="2" t="s">
         <v>274</v>
       </c>
+      <c r="D273" s="554" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="274" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="2" t="s">
         <v>275</v>
       </c>
+      <c r="D274" s="556" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="275" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
         <v>276</v>
       </c>
+      <c r="D275" s="558" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="276" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
         <v>277</v>
       </c>
+      <c r="D276" s="792" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="277" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
         <v>278</v>
       </c>
+      <c r="D277" s="562" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="278" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
         <v>279</v>
       </c>
+      <c r="D278" s="564" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="279" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="2" t="s">
         <v>280</v>
       </c>
+      <c r="D279" s="566" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="280" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="2" t="s">
         <v>281</v>
       </c>
+      <c r="D280" s="568" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="281" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="2" t="s">
         <v>282</v>
       </c>
+      <c r="D281" s="570" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="282" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="2" t="s">
         <v>283</v>
       </c>
+      <c r="D282" s="572" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="283" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="2" t="s">
         <v>284</v>
       </c>
+      <c r="D283" s="574" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="284" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="2" t="s">
         <v>285</v>
       </c>
+      <c r="D284" s="576" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="285" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="2" t="s">
         <v>286</v>
       </c>
+      <c r="D285" s="578" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="286" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="2" t="s">
         <v>287</v>
       </c>
+      <c r="D286" s="580" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="287" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="2" t="s">
         <v>288</v>
       </c>
+      <c r="D287" s="582" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="288" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="2" t="s">
         <v>289</v>
       </c>
+      <c r="D288" s="584" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="289" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
         <v>290</v>
       </c>
+      <c r="D289" s="586" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="290" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="2" t="s">
         <v>291</v>
       </c>
+      <c r="D290" s="588" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="291" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="2" t="s">
         <v>292</v>
       </c>
+      <c r="D291" s="590" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="292" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
         <v>293</v>
       </c>
+      <c r="D292" s="794" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="293" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="2" t="s">
         <v>294</v>
       </c>
+      <c r="D293" s="594" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="294" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="2" t="s">
         <v>295</v>
       </c>
+      <c r="D294" s="596" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="295" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="s">
         <v>296</v>
       </c>
+      <c r="D295" s="796" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="296" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="s">
         <v>297</v>
       </c>
+      <c r="D296" s="600" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="297" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="D297" s="798" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="298" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2" t="s">
         <v>299</v>
       </c>
+      <c r="D298" s="604" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="299" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2" t="s">
         <v>300</v>
       </c>
+      <c r="D299" s="606" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="300" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="2" t="s">
         <v>301</v>
       </c>
+      <c r="D300" s="608" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="301" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="2" t="s">
         <v>302</v>
       </c>
+      <c r="D301" s="610" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="302" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="2" t="s">
         <v>303</v>
       </c>
+      <c r="D302" s="612" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="303" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="2" t="s">
         <v>304</v>
       </c>
+      <c r="D303" s="614" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="304" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2" t="s">
         <v>305</v>
       </c>
+      <c r="D304" s="616" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="305" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="2" t="s">
         <v>306</v>
       </c>
+      <c r="D305" s="618" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="306" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="2" t="s">
         <v>307</v>
       </c>
+      <c r="D306" s="620" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="307" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="2" t="s">
         <v>308</v>
       </c>
+      <c r="D307" s="622" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="308" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="2" t="s">
         <v>309</v>
       </c>
+      <c r="D308" s="624" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="309" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="2" t="s">
         <v>310</v>
       </c>
+      <c r="D309" s="626" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="310" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="2" t="s">
         <v>311</v>
       </c>
+      <c r="D310" s="628" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="311" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="2" t="s">
         <v>312</v>
       </c>
+      <c r="D311" s="630" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="312" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="D312" s="632" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="313" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="2" t="s">
         <v>314</v>
       </c>
+      <c r="D313" s="634" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="314" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="2" t="s">
         <v>315</v>
       </c>
+      <c r="D314" s="636" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="315" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="2" t="s">
         <v>316</v>
       </c>
+      <c r="D315" s="638" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="316" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="2" t="s">
         <v>317</v>
       </c>
+      <c r="D316" s="640" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="317" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
         <v>318</v>
       </c>
+      <c r="D317" s="642" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="318" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
         <v>319</v>
       </c>
+      <c r="D318" s="644" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="319" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2" t="s">
         <v>320</v>
       </c>
+      <c r="D319" s="646" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="320" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="2" t="s">
         <v>321</v>
       </c>
+      <c r="D320" s="648" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="321" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="2" t="s">
         <v>322</v>
       </c>
+      <c r="D321" s="650" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="322" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="2" t="s">
         <v>323</v>
       </c>
+      <c r="D322" s="652" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="323" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="2" t="s">
         <v>324</v>
       </c>
+      <c r="D323" s="654" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="324" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="2" t="s">
         <v>325</v>
       </c>
+      <c r="D324" s="656" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="325" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="2" t="s">
         <v>326</v>
       </c>
+      <c r="D325" s="658" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="326" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
         <v>327</v>
       </c>
+      <c r="D326" s="660" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="327" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
         <v>328</v>
       </c>
+      <c r="D327" s="662" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="328" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
         <v>329</v>
       </c>
+      <c r="D328" s="664" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="329" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="2" t="s">
         <v>330</v>
       </c>
+      <c r="D329" s="666" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="330" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="2" t="s">
         <v>331</v>
       </c>
+      <c r="D330" s="668" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="331" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
         <v>332</v>
       </c>
+      <c r="D331" s="670" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="332" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
         <v>333</v>
       </c>
+      <c r="D332" s="672" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="333" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="2" t="s">
         <v>334</v>
       </c>
+      <c r="D333" s="674" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="334" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="2" t="s">
         <v>335</v>
       </c>
+      <c r="D334" s="676" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="335" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="2" t="s">
         <v>336</v>
       </c>
+      <c r="D335" s="678" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="336" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="2" t="s">
         <v>337</v>
       </c>
+      <c r="D336" s="680" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="337" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="2" t="s">
         <v>338</v>
       </c>
+      <c r="D337" s="682" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="338" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2" t="s">
         <v>339</v>
       </c>
+      <c r="D338" s="684" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="339" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
         <v>340</v>
       </c>
+      <c r="D339" s="686" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="340" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
         <v>341</v>
       </c>
+      <c r="D340" s="688" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="341" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
         <v>342</v>
       </c>
+      <c r="D341" s="690" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="342" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
         <v>343</v>
       </c>
+      <c r="D342" s="692" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="343" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
         <v>344</v>
       </c>
+      <c r="D343" s="694" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="344" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
         <v>345</v>
       </c>
+      <c r="D344" s="696" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="345" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
         <v>346</v>
       </c>
+      <c r="D345" s="698" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="346" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
         <v>347</v>
       </c>
+      <c r="D346" s="700" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="347" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
         <v>348</v>
       </c>
+      <c r="D347" s="702" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="348" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
         <v>349</v>
       </c>
+      <c r="D348" s="704" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="349" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
         <v>350</v>
       </c>
+      <c r="D349" s="706" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="350" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
         <v>351</v>
       </c>
+      <c r="D350" s="708" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="351" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
         <v>352</v>
       </c>
+      <c r="D351" s="710" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="352" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
         <v>353</v>
       </c>
+      <c r="D352" s="712" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="353" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
         <v>354</v>
       </c>
+      <c r="D353" s="714" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="354" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
         <v>355</v>
       </c>
+      <c r="D354" s="716" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="355" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
         <v>356</v>
       </c>
+      <c r="D355" s="718" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="356" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
         <v>357</v>
       </c>
+      <c r="D356" s="720" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="357" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
         <v>358</v>
       </c>
+      <c r="D357" s="722" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="358" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
         <v>359</v>
       </c>
+      <c r="D358" s="724" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="359" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
         <v>360</v>
       </c>
+      <c r="D359" s="726" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="360" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="D360" s="728" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="361" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
         <v>362</v>
       </c>
+      <c r="D361" s="730" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="362" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
         <v>363</v>
       </c>
+      <c r="D362" s="732" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="363" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
         <v>364</v>
       </c>
+      <c r="D363" s="734" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="364" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
         <v>365</v>
       </c>
+      <c r="D364" s="736" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="365" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="D365" s="738" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="366" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="2" t="s">
         <v>367</v>
       </c>
+      <c r="D366" s="740" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="367" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="2" t="s">
         <v>368</v>
       </c>
+      <c r="D367" s="742" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="368" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
         <v>369</v>
       </c>
+      <c r="D368" s="744" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="369" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
         <v>370</v>
       </c>
+      <c r="D369" s="746" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="370" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
         <v>371</v>
       </c>
+      <c r="D370" s="748" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="1"/>
@@ -3808,10 +6518,10 @@
       <c r="A1231" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <printOptions horizontalCentered="false" verticalCentered="false" headings="false" gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555" footer="0.51180555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <headerFooter differentOddEven="false" differentFirst="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>

</xml_diff>